<commit_message>
update li19 final model
</commit_message>
<xml_diff>
--- a/Collaborators/lj/Li19结果.xlsx
+++ b/Collaborators/lj/Li19结果.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Material-Studio\Collaborators\lj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18732CEA-D977-4466-B946-573ED08B6B0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A900892-D436-4DFB-BD7F-19373BAB7D1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14158" yWindow="1101" windowWidth="17425" windowHeight="9052" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13033" yWindow="1186" windowWidth="17425" windowHeight="9051" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="15">
   <si>
     <t>E/Ha</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -59,19 +60,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>bag1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>harvest</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>kettle</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>以上都重算</t>
+    <t>no smearing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>triangle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bag</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>计算方法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对17，8，13，6，1高精度优化</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fine+全电子相对论</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -408,27 +421,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3:K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.95" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -451,10 +469,22 @@
         <v>4</v>
       </c>
       <c r="H2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -462,16 +492,31 @@
         <v>-142.74326490000001</v>
       </c>
       <c r="E3">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="F3">
-        <v>-142.83940319999999</v>
+        <v>-142.74884610000001</v>
       </c>
       <c r="G3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>-142.74884610000001</v>
+      </c>
+      <c r="J3">
+        <v>17</v>
+      </c>
+      <c r="K3">
+        <v>-142.76005309999999</v>
+      </c>
+      <c r="L3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -479,16 +524,28 @@
         <v>-142.73332959999999</v>
       </c>
       <c r="E4">
-        <v>202</v>
+        <v>11</v>
       </c>
       <c r="F4">
-        <v>-142.83910639999999</v>
+        <v>-142.74878050000001</v>
       </c>
       <c r="G4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>-142.74878050000001</v>
+      </c>
+      <c r="J4">
+        <v>8</v>
+      </c>
+      <c r="K4">
+        <v>-142.75334720000001</v>
+      </c>
+      <c r="L4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>8</v>
       </c>
@@ -496,16 +553,25 @@
         <v>-142.73251959999999</v>
       </c>
       <c r="E5">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="F5">
-        <v>-142.82633820000001</v>
+        <v>-142.8249093</v>
       </c>
       <c r="G5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="H5">
+        <v>-142.74871400000001</v>
+      </c>
+      <c r="J5">
+        <v>13</v>
+      </c>
+      <c r="K5">
+        <v>-142.76035250000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>7</v>
       </c>
@@ -513,16 +579,25 @@
         <v>-142.7322308</v>
       </c>
       <c r="E6">
-        <v>122</v>
+        <v>3</v>
       </c>
       <c r="F6">
-        <v>-142.82580680000001</v>
+        <v>-142.82449130000001</v>
       </c>
       <c r="G6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <v>-142.74851509999999</v>
+      </c>
+      <c r="J6">
+        <v>6</v>
+      </c>
+      <c r="K6">
+        <v>-142.7498233</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -530,16 +605,25 @@
         <v>-142.7306122</v>
       </c>
       <c r="E7">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="F7">
-        <v>-142.82539990000001</v>
+        <v>-142.82318770000001</v>
       </c>
       <c r="G7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="H7">
+        <v>-142.74841219999999</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>-142.74892929999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -547,13 +631,19 @@
         <v>-142.72598669999999</v>
       </c>
       <c r="E8">
-        <v>110</v>
+        <v>14</v>
       </c>
       <c r="F8">
-        <v>-142.8249093</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-142.74813169999999</v>
+      </c>
+      <c r="G8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8">
+        <v>-142.74813169999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
@@ -561,13 +651,19 @@
         <v>-142.698736</v>
       </c>
       <c r="E9">
-        <v>8</v>
+        <v>129</v>
       </c>
       <c r="F9">
-        <v>-142.82490659999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-142.8245703</v>
+      </c>
+      <c r="G9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9">
+        <v>-142.7472047</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
@@ -575,13 +671,19 @@
         <v>-142.68770280000001</v>
       </c>
       <c r="E10">
-        <v>129</v>
+        <v>8</v>
       </c>
       <c r="F10">
-        <v>-142.8245703</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-142.82490659999999</v>
+      </c>
+      <c r="G10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10">
+        <v>-142.7392936</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
@@ -589,13 +691,19 @@
         <v>-142.377129</v>
       </c>
       <c r="E11">
-        <v>3</v>
+        <v>102</v>
       </c>
       <c r="F11">
-        <v>-142.82449130000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-142.82539990000001</v>
+      </c>
+      <c r="G11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11">
+        <v>-142.73859880000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5</v>
       </c>
@@ -603,180 +711,225 @@
         <v>-141.9059695</v>
       </c>
       <c r="E12">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="F12">
-        <v>-142.8236637</v>
+        <v>-142.82580680000001</v>
       </c>
       <c r="G12" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <v>-142.7385534</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E13">
+        <v>16</v>
+      </c>
+      <c r="F13">
+        <v>-142.7384289</v>
+      </c>
+      <c r="G13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13">
+        <v>-142.7384289</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>13</v>
+      </c>
+      <c r="F14">
+        <v>-142.738077</v>
+      </c>
+      <c r="G14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14">
+        <v>-142.738077</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>116</v>
+      </c>
+      <c r="F15">
+        <v>-142.8236637</v>
+      </c>
+      <c r="G15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15">
+        <v>-142.73789249999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>6</v>
+      </c>
+      <c r="F16">
+        <v>-142.83940319999999</v>
+      </c>
+      <c r="G16" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16">
+        <v>-142.7365887</v>
+      </c>
+    </row>
+    <row r="17" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E17">
         <v>1</v>
       </c>
-      <c r="F13">
+      <c r="F17">
         <v>-142.8232003</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E14">
-        <v>105</v>
-      </c>
-      <c r="F14">
-        <v>-142.82318770000001</v>
-      </c>
-      <c r="G14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E15">
+      <c r="G17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17">
+        <v>-142.7357379</v>
+      </c>
+    </row>
+    <row r="18" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>15</v>
+      </c>
+      <c r="F18">
+        <v>-142.73333550000001</v>
+      </c>
+      <c r="H18">
+        <v>-142.73333550000001</v>
+      </c>
+    </row>
+    <row r="19" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>12</v>
+      </c>
+      <c r="F19">
+        <v>-142.7276114</v>
+      </c>
+      <c r="H19">
+        <v>-142.7276114</v>
+      </c>
+    </row>
+    <row r="20" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>19</v>
+      </c>
+      <c r="F20">
+        <v>-142.7207602</v>
+      </c>
+      <c r="H20">
+        <v>-142.7207602</v>
+      </c>
+    </row>
+    <row r="21" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>20</v>
+      </c>
+      <c r="F21">
+        <v>-142.69427569999999</v>
+      </c>
+      <c r="H21">
+        <v>-142.69427569999999</v>
+      </c>
+    </row>
+    <row r="22" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>101</v>
+      </c>
+      <c r="F22">
+        <v>-142.80443260000001</v>
+      </c>
+    </row>
+    <row r="23" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>103</v>
+      </c>
+      <c r="F23">
+        <v>-142.82633820000001</v>
+      </c>
+      <c r="G23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E24">
         <v>104</v>
       </c>
-      <c r="F15">
+      <c r="F24">
         <v>-142.8218646</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E16">
+      <c r="G24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>106</v>
+      </c>
+      <c r="F25">
+        <v>-142.8202694</v>
+      </c>
+    </row>
+    <row r="26" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E26">
         <v>111</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F26" s="1">
         <v>-142.82137399999999</v>
       </c>
-      <c r="H16" t="s">
+      <c r="G26" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E17">
-        <v>106</v>
-      </c>
-      <c r="F17">
-        <v>-142.8202694</v>
-      </c>
-    </row>
-    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E18">
+    <row r="27" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <v>112</v>
+      </c>
+      <c r="F27">
+        <v>-142.81189560000001</v>
+      </c>
+    </row>
+    <row r="28" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E28">
         <v>113</v>
       </c>
-      <c r="F18">
+      <c r="F28">
         <v>-142.8190295</v>
       </c>
-      <c r="G18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E19">
+      <c r="G28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E29">
         <v>117</v>
       </c>
-      <c r="F19">
+      <c r="F29">
         <v>-142.8138496</v>
       </c>
     </row>
-    <row r="20" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E20">
-        <v>112</v>
-      </c>
-      <c r="F20">
-        <v>-142.81189560000001</v>
-      </c>
-    </row>
-    <row r="21" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E21">
-        <v>201</v>
-      </c>
-      <c r="F21">
-        <v>-142.8100335</v>
-      </c>
-      <c r="G21" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E22">
+    <row r="30" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E30">
         <v>118</v>
       </c>
-      <c r="F22">
+      <c r="F30">
         <v>-142.80444230000001</v>
       </c>
     </row>
-    <row r="23" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E23">
-        <v>101</v>
-      </c>
-      <c r="F23">
-        <v>-142.80443260000001</v>
-      </c>
-    </row>
-    <row r="24" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E24">
-        <v>127</v>
-      </c>
-      <c r="F24">
-        <v>-142.7957887</v>
-      </c>
-    </row>
-    <row r="25" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E25">
-        <v>128</v>
-      </c>
-      <c r="F25">
-        <v>-142.78471759999999</v>
-      </c>
-    </row>
-    <row r="26" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E26">
-        <v>124</v>
-      </c>
-      <c r="F26">
-        <v>-142.7802925</v>
-      </c>
-    </row>
-    <row r="27" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E27">
-        <v>126</v>
-      </c>
-      <c r="F27">
-        <v>-142.77586170000001</v>
-      </c>
-    </row>
-    <row r="28" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E28">
-        <v>132</v>
-      </c>
-      <c r="F28">
-        <v>-142.77216490000001</v>
-      </c>
-    </row>
-    <row r="29" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E29">
-        <v>203</v>
-      </c>
-      <c r="F29">
-        <v>-142.7659294</v>
-      </c>
-    </row>
-    <row r="30" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E30">
-        <v>125</v>
-      </c>
-      <c r="F30">
-        <v>-142.7655547</v>
-      </c>
-    </row>
-    <row r="31" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E31">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="F31">
-        <v>-142.7506401</v>
-      </c>
-    </row>
-    <row r="32" spans="5:7" x14ac:dyDescent="0.25">
+        <v>-142.7406699</v>
+      </c>
+    </row>
+    <row r="32" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E32">
         <v>121</v>
       </c>
@@ -784,7 +937,7 @@
         <v>-142.74795560000001</v>
       </c>
     </row>
-    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E33">
         <v>123</v>
       </c>
@@ -792,43 +945,122 @@
         <v>-142.7439114</v>
       </c>
     </row>
-    <row r="34" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E34">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="F34">
-        <v>-142.7406699</v>
-      </c>
-    </row>
-    <row r="35" spans="5:6" x14ac:dyDescent="0.25">
+        <v>-142.7802925</v>
+      </c>
+    </row>
+    <row r="35" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E35">
+        <v>125</v>
+      </c>
+      <c r="F35">
+        <v>-142.7655547</v>
+      </c>
+    </row>
+    <row r="36" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <v>126</v>
+      </c>
+      <c r="F36">
+        <v>-142.77586170000001</v>
+      </c>
+    </row>
+    <row r="37" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <v>127</v>
+      </c>
+      <c r="F37">
+        <v>-142.7957887</v>
+      </c>
+    </row>
+    <row r="38" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <v>128</v>
+      </c>
+      <c r="F38">
+        <v>-142.78471759999999</v>
+      </c>
+    </row>
+    <row r="39" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <v>130</v>
+      </c>
+      <c r="F39">
+        <v>-142.7506401</v>
+      </c>
+    </row>
+    <row r="40" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <v>131</v>
+      </c>
+      <c r="F40">
+        <v>-142.57031420000001</v>
+      </c>
+    </row>
+    <row r="41" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <v>132</v>
+      </c>
+      <c r="F41">
+        <v>-142.77216490000001</v>
+      </c>
+    </row>
+    <row r="42" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E42">
+        <v>133</v>
+      </c>
+      <c r="F42">
+        <v>-142.72353699999999</v>
+      </c>
+    </row>
+    <row r="43" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E43">
         <v>200</v>
       </c>
-      <c r="F35">
+      <c r="F43">
         <v>-142.73594299999999</v>
       </c>
     </row>
-    <row r="36" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E36">
-        <v>133</v>
-      </c>
-      <c r="F36">
-        <v>-142.72353699999999</v>
-      </c>
-    </row>
-    <row r="37" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E37">
-        <v>131</v>
-      </c>
-      <c r="F37">
-        <v>-142.57031420000001</v>
+    <row r="44" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E44">
+        <v>201</v>
+      </c>
+      <c r="F44">
+        <v>-142.8100335</v>
+      </c>
+      <c r="G44" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E45">
+        <v>202</v>
+      </c>
+      <c r="F45">
+        <v>-142.83910639999999</v>
+      </c>
+      <c r="G45" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E46">
+        <v>203</v>
+      </c>
+      <c r="F46">
+        <v>-142.7659294</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="E3:G37">
-    <sortCondition ref="F3:F37"/>
+  <sortState ref="E3:H46">
+    <sortCondition ref="H3:H46"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>